<commit_message>
Added Conditional based checklist rendering and added extraction logic choosing button
</commit_message>
<xml_diff>
--- a/Model_Series.xlsx
+++ b/Model_Series.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29609"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etihad-rail-poc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CFEA010-5616-478B-84A6-771C0817C625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFE4254F-8BF6-4B7C-97DF-2FF0D2575DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29400" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picklist Combined" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Category</t>
   </si>
@@ -82,28 +93,25 @@
     <t>CCTV System</t>
   </si>
   <si>
+    <t>Network Camera</t>
+  </si>
+  <si>
+    <t>NM-C110; NM-C130FD; NM-C150SD</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>Lite Series IP Cameras; Pro Series IP Cameras; PTZ Series; NVR 4000 Series</t>
+  </si>
+  <si>
     <t>IP CCTV System</t>
   </si>
   <si>
-    <t>Hikvision</t>
-  </si>
-  <si>
-    <t>IP Dome Camera Series; IP Bullet Camera Series; PTZ Camera Series; NVR 7600 Series</t>
-  </si>
-  <si>
-    <t>Dahua</t>
-  </si>
-  <si>
-    <t>Lite Series IP Cameras; Pro Series IP Cameras; PTZ Series; NVR 4000 Series</t>
-  </si>
-  <si>
     <t>Axis</t>
   </si>
   <si>
     <t>M Series (Fixed); P Series (Professional); Q Series (High-End); Axis Camera Station NVR</t>
-  </si>
-  <si>
-    <t>Bosch</t>
   </si>
   <si>
     <t>FLEXIDOME IP; DINION IP; AUTODOME PTZ; DIVAR Network Recorder</t>
@@ -143,12 +151,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -479,18 +487,18 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.899999999999999"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="4" width="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -532,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -546,7 +554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -560,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -574,7 +582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -588,7 +596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -602,7 +610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -616,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -624,13 +632,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -638,18 +646,18 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -658,74 +666,74 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Category additiion and openai extraction logic improvement
</commit_message>
<xml_diff>
--- a/Model_Series.xlsx
+++ b/Model_Series.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFE4254F-8BF6-4B7C-97DF-2FF0D2575DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etihad-rail-poc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB89782-3391-497F-8AE1-B801DE9DFD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29400" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picklist Combined" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Category</t>
   </si>
@@ -145,6 +148,15 @@
   </si>
   <si>
     <t>EST3; EST3X; iO-Series Panel; EST4</t>
+  </si>
+  <si>
+    <t>Packaged Air Conditioner</t>
+  </si>
+  <si>
+    <t>SKM</t>
+  </si>
+  <si>
+    <t>APMR-A</t>
   </si>
 </sst>
 </file>
@@ -484,17 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.899999999999999"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.625" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="97" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,16 +638,16 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -646,10 +658,10 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -657,13 +669,13 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -674,24 +686,24 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -702,10 +714,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -716,10 +728,10 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -730,9 +742,23 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>